<commit_message>
Correção Modelagem Coluna Fonte
</commit_message>
<xml_diff>
--- a/Modelagem/Dicionário de Dados.xlsx
+++ b/Modelagem/Dicionário de Dados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Desktop\TCC\Modelagem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eduar\Desktop\TCC\portal-transparencia-Emurb\Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A766E8-E34A-4962-80B8-A5DC470425F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460A5DA4-249C-4C3A-9C59-D0082436F685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{6F74207C-FE9B-4F55-9170-6BDF66C58CA2}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="88">
   <si>
     <t>TIPO</t>
   </si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>Identificador para o credor (Número Aleatório)</t>
+  </si>
+  <si>
+    <t>Anulação</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1207,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1417,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>71</v>
@@ -1583,7 +1586,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1815,7 +1818,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>71</v>

</xml_diff>